<commit_message>
More tweaks to date-of-death states
</commit_message>
<xml_diff>
--- a/notebooks/DateOfDeath.xlsx
+++ b/notebooks/DateOfDeath.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrick/dev/covid/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1E2C95-E252-DE44-9E3F-62B8F6A1568D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7751AB-8388-9544-86A2-06F44842B818}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{20D733EF-6676-F449-AF32-307F4FADCE6E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10000" windowHeight="21000" activeTab="1" xr2:uid="{20D733EF-6676-F449-AF32-307F4FADCE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Arizona" sheetId="1" r:id="rId1"/>
@@ -413,11 +413,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C77E57-C0B4-9B4C-98EA-985C0D327C7F}">
-  <dimension ref="A1:C328"/>
+  <dimension ref="A1:C329"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A322" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A329" sqref="A329"/>
+      <pane ySplit="1" topLeftCell="A304" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B318" sqref="B318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4157,11 +4157,11 @@
         <v>44201</v>
       </c>
       <c r="B312">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C312" s="4">
         <f t="shared" si="4"/>
-        <v>10837</v>
+        <v>10838</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.2">
@@ -4173,7 +4173,7 @@
       </c>
       <c r="C313" s="4">
         <f t="shared" si="4"/>
-        <v>10946</v>
+        <v>10947</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.2">
@@ -4181,11 +4181,11 @@
         <v>44203</v>
       </c>
       <c r="B314">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C314" s="4">
         <f t="shared" si="4"/>
-        <v>11058</v>
+        <v>11061</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.2">
@@ -4193,11 +4193,11 @@
         <v>44204</v>
       </c>
       <c r="B315">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C315" s="4">
         <f t="shared" si="4"/>
-        <v>11182</v>
+        <v>11188</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.2">
@@ -4205,11 +4205,11 @@
         <v>44205</v>
       </c>
       <c r="B316">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C316" s="4">
         <f t="shared" si="4"/>
-        <v>11298</v>
+        <v>11308</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.2">
@@ -4217,11 +4217,11 @@
         <v>44206</v>
       </c>
       <c r="B317">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C317" s="4">
         <f t="shared" si="4"/>
-        <v>11415</v>
+        <v>11427</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.2">
@@ -4229,11 +4229,11 @@
         <v>44207</v>
       </c>
       <c r="B318">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C318" s="4">
         <f t="shared" si="4"/>
-        <v>11510</v>
+        <v>11528</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.2">
@@ -4241,11 +4241,11 @@
         <v>44208</v>
       </c>
       <c r="B319">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C319" s="4">
         <f t="shared" si="4"/>
-        <v>11615</v>
+        <v>11634</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.2">
@@ -4253,11 +4253,11 @@
         <v>44209</v>
       </c>
       <c r="B320">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C320" s="4">
         <f t="shared" si="4"/>
-        <v>11725</v>
+        <v>11746</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.2">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="C321" s="4">
         <f t="shared" si="4"/>
-        <v>11824</v>
+        <v>11845</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.2">
@@ -4277,11 +4277,11 @@
         <v>44211</v>
       </c>
       <c r="B322">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C322" s="4">
         <f t="shared" si="4"/>
-        <v>11907</v>
+        <v>11932</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.2">
@@ -4289,11 +4289,11 @@
         <v>44212</v>
       </c>
       <c r="B323">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C323" s="4">
         <f t="shared" si="4"/>
-        <v>11963</v>
+        <v>11989</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.2">
@@ -4301,11 +4301,11 @@
         <v>44213</v>
       </c>
       <c r="B324">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C324" s="4">
-        <f t="shared" ref="C324:C328" si="5">C323+B324</f>
-        <v>12023</v>
+        <f t="shared" ref="C324:C329" si="5">C323+B324</f>
+        <v>12057</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.2">
@@ -4313,11 +4313,11 @@
         <v>44214</v>
       </c>
       <c r="B325">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C325" s="4">
         <f t="shared" si="5"/>
-        <v>12085</v>
+        <v>12123</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.2">
@@ -4325,11 +4325,11 @@
         <v>44215</v>
       </c>
       <c r="B326">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C326" s="4">
         <f t="shared" si="5"/>
-        <v>12124</v>
+        <v>12171</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.2">
@@ -4337,11 +4337,11 @@
         <v>44216</v>
       </c>
       <c r="B327">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C327" s="4">
         <f t="shared" si="5"/>
-        <v>12140</v>
+        <v>12201</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.2">
@@ -4349,11 +4349,23 @@
         <v>44217</v>
       </c>
       <c r="B328">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C328" s="4">
         <f t="shared" si="5"/>
-        <v>12142</v>
+        <v>12207</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A329" s="2">
+        <v>44218</v>
+      </c>
+      <c r="B329">
+        <v>2</v>
+      </c>
+      <c r="C329" s="4">
+        <f t="shared" si="5"/>
+        <v>12209</v>
       </c>
     </row>
   </sheetData>
@@ -4366,8 +4378,8 @@
   <dimension ref="A1:E326"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A299" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D309" sqref="D309"/>
+      <pane ySplit="1" topLeftCell="A301" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C311" sqref="C311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>